<commit_message>
New option LoadSheets, overhaul of tests etc.
Sheets new load automatically unless you set the LoadSheets option to
false. Tests have been divided into classes for different
configurations. A serious bug was fixed in Sheets.Open(). Other minor
improvements.
</commit_message>
<xml_diff>
--- a/ExcelLibrary/ExcelLibrary.Tests/Input/test1.xlsx
+++ b/ExcelLibrary/ExcelLibrary.Tests/Input/test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11835"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14565" windowHeight="10860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Banana</t>
   </si>
@@ -32,16 +32,139 @@
   </si>
   <si>
     <t>Melon</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>Scientific</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>The default number format that Excel applies when you type a number. For the most part, numbers that are formatted with the General format are displayed just the way you type them. However, if the cell is not wide enough to show the entire number, the General format rounds the numbers with decimals. The General number format also uses scientific (exponential) notation for large numbers (12 or more digits).</t>
+  </si>
+  <si>
+    <t>Used for the general display of numbers. You can specify the number of decimal places that you want to use, whether you want to use a thousands separator, and how you want to display negative numbers.</t>
+  </si>
+  <si>
+    <t>Used for general monetary values and displays the default currency symbol with numbers. You can specify the number of decimal places that you want to use, whether you want to use a thousands separator, and how you want to display negative numbers.</t>
+  </si>
+  <si>
+    <t>Also used for monetary values, but it aligns the currency symbols and decimal points of numbers in a column.</t>
+  </si>
+  <si>
+    <t>Displays date and time serial numbers as date values, according to the type and locale (location) that you specify. Date formats that begin with an asterisk (*) respond to changes in regional date and time settings that are specified in Control Panel. Formats without an asterisk are not affected by Control Panel settings.</t>
+  </si>
+  <si>
+    <t>Displays date and time serial numbers as time values, according to the type and locale (location) that you specify. Time formats that begin with an asterisk (*) respond to changes in regional date and time settings that are specified in Control Panel. Formats without an asterisk are not affected by Control Panel settings.</t>
+  </si>
+  <si>
+    <t>Multiplies the cell value by 100 and displays the result with a percent (%) symbol. You can specify the number of decimal places that you want to use.</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Displays a number as a fraction, according to the type of fraction that you specify.</t>
+  </si>
+  <si>
+    <t>Displays a number in exponential notation, replacing part of the number with E+n, where E (which stands for Exponent) multiplies the preceding number by 10 to the nth power. For example, a 2-decimal Scientific format displays 12345678901 as 1.23E+10, which is 1.23 times 10 to the 10th power. You can specify the number of decimal places that you want to use.</t>
+  </si>
+  <si>
+    <t>Treats the content of a cell as text and displays the content exactly as you type it, even when you type numbers.</t>
+  </si>
+  <si>
+    <t>Displays a number as a postal code (ZIP Code), phone number, or Social Security number.</t>
+  </si>
+  <si>
+    <t>Allows you to modify a copy of an existing number format code. Use this format to create a custom number format that is added to the list of number format codes. You can add between 200 and 250 custom number formats, depending on the language version of Excel that is installed on your computer.</t>
+  </si>
+  <si>
+    <t>räksmörgås</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Expected string output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="000\ 00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;kr&quot;"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -55,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,24 +186,219 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="12" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3262303" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3733800" y="257175"/>
+          <a:ext cx="3262303" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCC66"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This sheet is used for tests relating to finding cell data</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>on</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> a sheet. Some data is hidden.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3321935" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6562725" y="352425"/>
+          <a:ext cx="3321935" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCC66"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This sheet is used for tests relating to number formats.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -379,6 +697,11 @@
     <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>123.45</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
@@ -406,18 +729,210 @@
     <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7">
+        <v>123</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8">
+        <v>123.45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9">
+        <v>123.45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10">
+        <v>123.45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="11">
+        <v>42369</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4">
+        <v>42369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.89054398148148151</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.89054398148148151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.67</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="14">
+        <v>12300000000</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12300000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="15">
+        <v>19161</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1">
+        <v>19161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>